<commit_message>
add part b to exercise and organize part a folder
</commit_message>
<xml_diff>
--- a/sea_navigation/sites_map.xlsx
+++ b/sea_navigation/sites_map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\borges\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borges\PycharmProjects\optimization-cases\sea_navigation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>x</t>
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>island_y_bottom_right</t>
+  </si>
+  <si>
+    <t>island_x_bottom_right</t>
+  </si>
+  <si>
+    <t>island_x_bottom_left</t>
+  </si>
+  <si>
+    <t>island_y_bottom_left</t>
+  </si>
+  <si>
+    <t>island_x_top_right</t>
+  </si>
+  <si>
+    <t>island_y_top_right</t>
+  </si>
+  <si>
+    <t>island_x_top_left</t>
+  </si>
+  <si>
+    <t>island_y_top_left</t>
   </si>
 </sst>
 </file>
@@ -119,7 +143,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -149,7 +173,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8374CBB7-8DEA-4A23-B56A-FA91EA3C7847}" type="CELLRANGE">
+                    <a:fld id="{9C0ABBE6-AF15-44DA-A890-793AE8BF0DDD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -185,7 +209,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B3B047A-5291-46EF-BD94-607B80F615E4}" type="CELLRANGE">
+                    <a:fld id="{854F665C-6160-460D-934F-4F4E1A04E594}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -221,7 +245,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E928122-0261-4E32-9703-C0ECDBA0614A}" type="CELLRANGE">
+                    <a:fld id="{7A250E3A-FDEA-4B34-95B7-38FC2FAFA338}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -251,13 +275,53 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.4912510936133497E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{6B065E2C-2F52-4ACF-94C5-D5083250CC03}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-2853-4575-819A-05F7E4BE37BC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
               <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75FB3DFB-07D8-418E-B944-E12BCE541C7A}" type="CELLRANGE">
+                    <a:fld id="{379229C8-05D1-4555-8317-421E3AF851E1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -281,19 +345,19 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-2853-4575-819A-05F7E4BE37BC}"/>
+                  <c16:uniqueId val="{00000006-2853-4575-819A-05F7E4BE37BC}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="4"/>
+              <c:idx val="5"/>
               <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{004CA0F8-007B-45E2-B096-2EED76D6D092}" type="CELLRANGE">
+                    <a:fld id="{A78E86EC-45FE-4AC7-AF7E-11F40DD2B8C1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -317,19 +381,19 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-2853-4575-819A-05F7E4BE37BC}"/>
+                  <c16:uniqueId val="{00000007-2853-4575-819A-05F7E4BE37BC}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="5"/>
+              <c:idx val="6"/>
               <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{39F4FB85-CF63-41A5-BE50-0D0881F388C4}" type="CELLRANGE">
+                    <a:fld id="{1A7D1513-BBE5-4626-90B5-5F1A1A8FA6BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -353,19 +417,19 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-2853-4575-819A-05F7E4BE37BC}"/>
+                  <c16:uniqueId val="{00000008-2853-4575-819A-05F7E4BE37BC}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="6"/>
+              <c:idx val="7"/>
               <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BF04530D-DDE3-4503-911D-AD77CAADEF88}" type="CELLRANGE">
+                    <a:fld id="{1966BB5D-985F-4568-92B9-7D0FF35675E9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -389,19 +453,19 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-2853-4575-819A-05F7E4BE37BC}"/>
+                  <c16:uniqueId val="{00000009-2853-4575-819A-05F7E4BE37BC}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="7"/>
+              <c:idx val="8"/>
               <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{62429FDA-76DB-4C70-BB68-C38A22A26684}" type="CELLRANGE">
+                    <a:fld id="{89E83015-84D3-4953-AC1A-769C573504C4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -425,19 +489,19 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-2853-4575-819A-05F7E4BE37BC}"/>
+                  <c16:uniqueId val="{0000000A-2853-4575-819A-05F7E4BE37BC}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="8"/>
+              <c:idx val="9"/>
               <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{71EA0B70-D233-418B-9EE0-3B69167F98C5}" type="CELLRANGE">
+                    <a:fld id="{9DAF598E-A855-44D2-B2FF-1690A1A0A0EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -461,19 +525,19 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-2853-4575-819A-05F7E4BE37BC}"/>
+                  <c16:uniqueId val="{0000000B-2853-4575-819A-05F7E4BE37BC}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="9"/>
+              <c:idx val="10"/>
               <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6514B478-F2A7-46F4-80FE-2BDF2FF6704A}" type="CELLRANGE">
+                    <a:fld id="{EC1E62CA-264A-457A-B7A5-852A48C27CFE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -497,19 +561,19 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000B-2853-4575-819A-05F7E4BE37BC}"/>
+                  <c16:uniqueId val="{0000000C-2853-4575-819A-05F7E4BE37BC}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="10"/>
+              <c:idx val="11"/>
               <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{00BA9474-36FA-4F9F-B682-F10A3645050E}" type="CELLRANGE">
+                    <a:fld id="{191D853C-515A-4D1F-9785-FA3268D6220D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -533,19 +597,19 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000C-2853-4575-819A-05F7E4BE37BC}"/>
+                  <c16:uniqueId val="{0000000D-2853-4575-819A-05F7E4BE37BC}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="11"/>
+              <c:idx val="12"/>
               <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A42B8152-E83D-4447-8533-523D097E4224}" type="CELLRANGE">
+                    <a:fld id="{E056E4FB-45C6-4EE4-BD8F-49CF0C9BA763}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -569,19 +633,59 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000D-2853-4575-819A-05F7E4BE37BC}"/>
+                  <c16:uniqueId val="{0000000E-2853-4575-819A-05F7E4BE37BC}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
-              <c:idx val="12"/>
+              <c:idx val="13"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.4076771653543357E-2"/>
+                  <c:y val="5.5555555555555552E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{225AFE4B-27BA-4CF9-9CAF-7BF18B2ACF41}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-2853-4575-819A-05F7E4BE37BC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
               <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36DFA633-530D-40E3-9A69-21CE83D0280E}" type="CELLRANGE">
+                    <a:fld id="{A4D80E3B-5E56-40E6-972E-AD3E6A15BED9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -605,78 +709,6 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000E-2853-4575-819A-05F7E4BE37BC}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="13"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{1F7134BB-876B-4175-A1E8-CA9B75576261}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="l"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000F-2853-4575-819A-05F7E4BE37BC}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="14"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{6061E251-E5EF-462F-8EA9-9953C63AA8A2}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
-                      <a:t>[CELLRANGE]</a:t>
-                    </a:fld>
-                    <a:endParaRPr lang="en-US"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:dLblPos val="l"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000010-2853-4575-819A-05F7E4BE37BC}"/>
                 </c:ext>
               </c:extLst>
@@ -689,7 +721,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F60F63B0-0368-40C0-8A72-C8DEDA13DAC9}" type="CELLRANGE">
+                    <a:fld id="{2FE95CE0-598F-4E56-A545-5F08C8EC462F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -956,6 +988,159 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>island</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.13947222222222222"/>
+                  <c:y val="-5.783573928258972E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-DC04-4B62-816B-F8CDB81CBB98}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Planilha1!$F$2,Planilha1!$F$4,Planilha1!$F$6,Planilha1!$F$8,Planilha1!$F$2)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Planilha1!$G$2,Planilha1!$G$4,Planilha1!$G$6,Planilha1!$G$8,Planilha1!$G$2)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DC04-4B62-816B-F8CDB81CBB98}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
@@ -972,6 +1157,8 @@
         <c:axId val="2125558975"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="110"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1027,13 +1214,15 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="2125560223"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="2125560223"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="110"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1089,7 +1278,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="2125558975"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1697,16 +1886,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1991,23 +2180,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2017,8 +2215,14 @@
       <c r="C2">
         <v>0</v>
       </c>
+      <c r="F2">
+        <v>38</v>
+      </c>
+      <c r="G2">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2028,8 +2232,14 @@
       <c r="C3">
         <v>10</v>
       </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2039,8 +2249,14 @@
       <c r="C4">
         <v>20</v>
       </c>
+      <c r="F4">
+        <v>35</v>
+      </c>
+      <c r="G4">
+        <v>42</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2050,8 +2266,14 @@
       <c r="C5">
         <v>30</v>
       </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2061,8 +2283,14 @@
       <c r="C6">
         <v>80</v>
       </c>
+      <c r="F6">
+        <v>39</v>
+      </c>
+      <c r="G6">
+        <v>70</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2072,8 +2300,14 @@
       <c r="C7">
         <v>50</v>
       </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2083,8 +2317,14 @@
       <c r="C8">
         <v>40</v>
       </c>
+      <c r="F8">
+        <v>44</v>
+      </c>
+      <c r="G8">
+        <v>58</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2095,7 +2335,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2106,7 +2346,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2117,7 +2357,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2128,7 +2368,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2139,7 +2379,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2150,7 +2390,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2161,7 +2401,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2185,6 +2425,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>